<commit_message>
reglage pb 0/1 NoOne
</commit_message>
<xml_diff>
--- a/src/loader_package/xlsx/america.xlsx
+++ b/src/loader_package/xlsx/america.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\ING3\Informatique\Projet\java_project_desautel_pellen_perold\src\loader_package\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154F5351-CB5C-47E3-B0A4-1081987CC64B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4D11C8-BE8C-4072-9991-AD365F028268}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="official" sheetId="4" r:id="rId4"/>
     <sheet name="election" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">elector!$A$1:$E$4000</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -17218,7 +17221,7 @@
   <dimension ref="A1:J4004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17228,7 +17231,7 @@
     <col min="3" max="3" width="17.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -38270,7 +38273,7 @@
         <v>1905</v>
       </c>
       <c r="F1002" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1003" spans="1:10" x14ac:dyDescent="0.3">
@@ -38350,7 +38353,7 @@
         <v>6</v>
       </c>
       <c r="F1006" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1007" spans="1:10" x14ac:dyDescent="0.3">
@@ -38470,7 +38473,7 @@
         <v>2</v>
       </c>
       <c r="F1012" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1013" spans="1:6" x14ac:dyDescent="0.3">
@@ -38790,7 +38793,7 @@
         <v>1905</v>
       </c>
       <c r="F1028" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1029" spans="1:6" x14ac:dyDescent="0.3">
@@ -38990,7 +38993,7 @@
         <v>2</v>
       </c>
       <c r="F1038" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1039" spans="1:6" x14ac:dyDescent="0.3">
@@ -39210,7 +39213,7 @@
         <v>1905</v>
       </c>
       <c r="F1049" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1050" spans="1:6" x14ac:dyDescent="0.3">
@@ -39410,7 +39413,7 @@
         <v>2</v>
       </c>
       <c r="F1059" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1060" spans="1:6" x14ac:dyDescent="0.3">
@@ -39690,7 +39693,7 @@
         <v>1905</v>
       </c>
       <c r="F1073" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1074" spans="1:6" x14ac:dyDescent="0.3">
@@ -39890,7 +39893,7 @@
         <v>2</v>
       </c>
       <c r="F1083" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1084" spans="1:6" x14ac:dyDescent="0.3">
@@ -40130,7 +40133,7 @@
         <v>1905</v>
       </c>
       <c r="F1095" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1096" spans="1:6" x14ac:dyDescent="0.3">
@@ -40330,7 +40333,7 @@
         <v>6</v>
       </c>
       <c r="F1105" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1106" spans="1:6" x14ac:dyDescent="0.3">
@@ -40550,7 +40553,7 @@
         <v>1905</v>
       </c>
       <c r="F1116" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1117" spans="1:6" x14ac:dyDescent="0.3">
@@ -40750,7 +40753,7 @@
         <v>2</v>
       </c>
       <c r="F1126" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1127" spans="1:6" x14ac:dyDescent="0.3">
@@ -41030,7 +41033,7 @@
         <v>1905</v>
       </c>
       <c r="F1140" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1141" spans="1:6" x14ac:dyDescent="0.3">
@@ -41230,7 +41233,7 @@
         <v>2</v>
       </c>
       <c r="F1150" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1151" spans="1:6" x14ac:dyDescent="0.3">
@@ -41330,7 +41333,7 @@
         <v>1905</v>
       </c>
       <c r="F1155" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1156" spans="1:6" x14ac:dyDescent="0.3">
@@ -41530,7 +41533,7 @@
         <v>2</v>
       </c>
       <c r="F1165" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1166" spans="1:6" x14ac:dyDescent="0.3">
@@ -41870,7 +41873,7 @@
         <v>1905</v>
       </c>
       <c r="F1182" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1183" spans="1:6" x14ac:dyDescent="0.3">
@@ -42070,7 +42073,7 @@
         <v>2</v>
       </c>
       <c r="F1192" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1193" spans="1:6" x14ac:dyDescent="0.3">
@@ -42350,7 +42353,7 @@
         <v>1905</v>
       </c>
       <c r="F1206" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1207" spans="1:6" x14ac:dyDescent="0.3">
@@ -42550,7 +42553,7 @@
         <v>6</v>
       </c>
       <c r="F1216" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1217" spans="1:6" x14ac:dyDescent="0.3">
@@ -42770,7 +42773,7 @@
         <v>1905</v>
       </c>
       <c r="F1227" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1228" spans="1:6" x14ac:dyDescent="0.3">
@@ -42970,7 +42973,7 @@
         <v>6</v>
       </c>
       <c r="F1237" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1238" spans="1:6" x14ac:dyDescent="0.3">
@@ -43010,7 +43013,7 @@
         <v>1905</v>
       </c>
       <c r="F1239" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1240" spans="1:6" x14ac:dyDescent="0.3">
@@ -43210,7 +43213,7 @@
         <v>2</v>
       </c>
       <c r="F1249" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1250" spans="1:6" x14ac:dyDescent="0.3">
@@ -43250,7 +43253,7 @@
         <v>1905</v>
       </c>
       <c r="F1251" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1252" spans="1:6" x14ac:dyDescent="0.3">
@@ -43430,7 +43433,7 @@
         <v>1905</v>
       </c>
       <c r="F1260" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1261" spans="1:6" x14ac:dyDescent="0.3">
@@ -43450,7 +43453,7 @@
         <v>2</v>
       </c>
       <c r="F1261" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1262" spans="1:6" x14ac:dyDescent="0.3">
@@ -43630,7 +43633,7 @@
         <v>2</v>
       </c>
       <c r="F1270" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1271" spans="1:6" x14ac:dyDescent="0.3">
@@ -43670,7 +43673,7 @@
         <v>1905</v>
       </c>
       <c r="F1272" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1273" spans="1:6" x14ac:dyDescent="0.3">
@@ -43870,7 +43873,7 @@
         <v>2</v>
       </c>
       <c r="F1282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1283" spans="1:6" x14ac:dyDescent="0.3">
@@ -43910,7 +43913,7 @@
         <v>1905</v>
       </c>
       <c r="F1284" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1285" spans="1:6" x14ac:dyDescent="0.3">
@@ -44110,7 +44113,7 @@
         <v>2</v>
       </c>
       <c r="F1294" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1295" spans="1:6" x14ac:dyDescent="0.3">
@@ -44150,7 +44153,7 @@
         <v>1905</v>
       </c>
       <c r="F1296" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1297" spans="1:6" x14ac:dyDescent="0.3">
@@ -44350,7 +44353,7 @@
         <v>6</v>
       </c>
       <c r="F1306" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1307" spans="1:6" x14ac:dyDescent="0.3">
@@ -44450,7 +44453,7 @@
         <v>1905</v>
       </c>
       <c r="F1311" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1312" spans="1:6" x14ac:dyDescent="0.3">
@@ -44650,7 +44653,7 @@
         <v>6</v>
       </c>
       <c r="F1321" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1322" spans="1:6" x14ac:dyDescent="0.3">
@@ -44690,7 +44693,7 @@
         <v>1905</v>
       </c>
       <c r="F1323" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1324" spans="1:6" x14ac:dyDescent="0.3">
@@ -44870,7 +44873,7 @@
         <v>1905</v>
       </c>
       <c r="F1332" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1333" spans="1:6" x14ac:dyDescent="0.3">
@@ -44890,7 +44893,7 @@
         <v>64</v>
       </c>
       <c r="F1333" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1334" spans="1:6" x14ac:dyDescent="0.3">
@@ -45070,7 +45073,7 @@
         <v>6</v>
       </c>
       <c r="F1342" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1343" spans="1:6" x14ac:dyDescent="0.3">
@@ -45230,7 +45233,7 @@
         <v>1905</v>
       </c>
       <c r="F1350" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1351" spans="1:6" x14ac:dyDescent="0.3">
@@ -45410,7 +45413,7 @@
         <v>1905</v>
       </c>
       <c r="F1359" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1360" spans="1:6" x14ac:dyDescent="0.3">
@@ -45430,7 +45433,7 @@
         <v>2</v>
       </c>
       <c r="F1360" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1361" spans="1:6" x14ac:dyDescent="0.3">
@@ -45610,7 +45613,7 @@
         <v>40</v>
       </c>
       <c r="F1369" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1370" spans="1:6" x14ac:dyDescent="0.3">
@@ -45650,7 +45653,7 @@
         <v>1905</v>
       </c>
       <c r="F1371" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1372" spans="1:6" x14ac:dyDescent="0.3">
@@ -45850,7 +45853,7 @@
         <v>6</v>
       </c>
       <c r="F1381" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1382" spans="1:6" x14ac:dyDescent="0.3">
@@ -45950,7 +45953,7 @@
         <v>1905</v>
       </c>
       <c r="F1386" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1387" spans="1:6" x14ac:dyDescent="0.3">
@@ -46150,7 +46153,7 @@
         <v>64</v>
       </c>
       <c r="F1396" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1397" spans="1:6" x14ac:dyDescent="0.3">
@@ -46190,7 +46193,7 @@
         <v>1905</v>
       </c>
       <c r="F1398" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1399" spans="1:6" x14ac:dyDescent="0.3">
@@ -46390,7 +46393,7 @@
         <v>2</v>
       </c>
       <c r="F1408" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1409" spans="1:6" x14ac:dyDescent="0.3">
@@ -46430,7 +46433,7 @@
         <v>1905</v>
       </c>
       <c r="F1410" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1411" spans="1:6" x14ac:dyDescent="0.3">
@@ -46610,7 +46613,7 @@
         <v>1905</v>
       </c>
       <c r="F1419" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1420" spans="1:6" x14ac:dyDescent="0.3">
@@ -46630,7 +46633,7 @@
         <v>64</v>
       </c>
       <c r="F1420" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1421" spans="1:6" x14ac:dyDescent="0.3">
@@ -46810,7 +46813,7 @@
         <v>2</v>
       </c>
       <c r="F1429" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1430" spans="1:6" x14ac:dyDescent="0.3">
@@ -46910,7 +46913,7 @@
         <v>1905</v>
       </c>
       <c r="F1434" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1435" spans="1:6" x14ac:dyDescent="0.3">
@@ -47110,7 +47113,7 @@
         <v>2</v>
       </c>
       <c r="F1444" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1445" spans="1:6" x14ac:dyDescent="0.3">
@@ -47210,7 +47213,7 @@
         <v>1905</v>
       </c>
       <c r="F1449" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1450" spans="1:6" x14ac:dyDescent="0.3">
@@ -47410,7 +47413,7 @@
         <v>2</v>
       </c>
       <c r="F1459" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1460" spans="1:6" x14ac:dyDescent="0.3">
@@ -47570,7 +47573,7 @@
         <v>1905</v>
       </c>
       <c r="F1467" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1468" spans="1:6" x14ac:dyDescent="0.3">
@@ -47770,7 +47773,7 @@
         <v>6</v>
       </c>
       <c r="F1477" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1478" spans="1:6" x14ac:dyDescent="0.3">
@@ -47870,7 +47873,7 @@
         <v>1905</v>
       </c>
       <c r="F1482" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1483" spans="1:6" x14ac:dyDescent="0.3">
@@ -48070,7 +48073,7 @@
         <v>2</v>
       </c>
       <c r="F1492" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1493" spans="1:6" x14ac:dyDescent="0.3">
@@ -48230,7 +48233,7 @@
         <v>1905</v>
       </c>
       <c r="F1500" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1501" spans="1:6" x14ac:dyDescent="0.3">
@@ -48430,7 +48433,7 @@
         <v>2</v>
       </c>
       <c r="F1510" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1511" spans="1:6" x14ac:dyDescent="0.3">
@@ -48590,7 +48593,7 @@
         <v>1905</v>
       </c>
       <c r="F1518" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1519" spans="1:6" x14ac:dyDescent="0.3">
@@ -48790,7 +48793,7 @@
         <v>2</v>
       </c>
       <c r="F1528" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1529" spans="1:6" x14ac:dyDescent="0.3">
@@ -48950,7 +48953,7 @@
         <v>1905</v>
       </c>
       <c r="F1536" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1537" spans="1:6" x14ac:dyDescent="0.3">
@@ -49150,7 +49153,7 @@
         <v>6</v>
       </c>
       <c r="F1546" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1547" spans="1:6" x14ac:dyDescent="0.3">
@@ -49250,7 +49253,7 @@
         <v>1905</v>
       </c>
       <c r="F1551" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1552" spans="1:6" x14ac:dyDescent="0.3">
@@ -49450,7 +49453,7 @@
         <v>2</v>
       </c>
       <c r="F1561" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1562" spans="1:6" x14ac:dyDescent="0.3">
@@ -49730,7 +49733,7 @@
         <v>1905</v>
       </c>
       <c r="F1575" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1576" spans="1:6" x14ac:dyDescent="0.3">
@@ -49930,7 +49933,7 @@
         <v>6</v>
       </c>
       <c r="F1585" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1586" spans="1:6" x14ac:dyDescent="0.3">
@@ -50090,7 +50093,7 @@
         <v>1905</v>
       </c>
       <c r="F1593" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1594" spans="1:6" x14ac:dyDescent="0.3">
@@ -50290,7 +50293,7 @@
         <v>64</v>
       </c>
       <c r="F1603" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1604" spans="1:6" x14ac:dyDescent="0.3">
@@ -50450,7 +50453,7 @@
         <v>1905</v>
       </c>
       <c r="F1611" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1612" spans="1:6" x14ac:dyDescent="0.3">
@@ -50650,7 +50653,7 @@
         <v>6</v>
       </c>
       <c r="F1621" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1622" spans="1:6" x14ac:dyDescent="0.3">
@@ -50810,7 +50813,7 @@
         <v>1905</v>
       </c>
       <c r="F1629" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1630" spans="1:6" x14ac:dyDescent="0.3">
@@ -51010,7 +51013,7 @@
         <v>6</v>
       </c>
       <c r="F1639" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1640" spans="1:6" x14ac:dyDescent="0.3">
@@ -51290,7 +51293,7 @@
         <v>1905</v>
       </c>
       <c r="F1653" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1654" spans="1:6" x14ac:dyDescent="0.3">
@@ -51490,7 +51493,7 @@
         <v>2</v>
       </c>
       <c r="F1663" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1664" spans="1:6" x14ac:dyDescent="0.3">
@@ -51770,7 +51773,7 @@
         <v>1905</v>
       </c>
       <c r="F1677" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1678" spans="1:6" x14ac:dyDescent="0.3">
@@ -51970,7 +51973,7 @@
         <v>6</v>
       </c>
       <c r="F1687" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1688" spans="1:6" x14ac:dyDescent="0.3">
@@ -52250,7 +52253,7 @@
         <v>1905</v>
       </c>
       <c r="F1701" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1702" spans="1:6" x14ac:dyDescent="0.3">
@@ -52450,7 +52453,7 @@
         <v>2</v>
       </c>
       <c r="F1711" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1712" spans="1:6" x14ac:dyDescent="0.3">
@@ -52670,7 +52673,7 @@
         <v>1905</v>
       </c>
       <c r="F1722" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1723" spans="1:6" x14ac:dyDescent="0.3">
@@ -52870,7 +52873,7 @@
         <v>6</v>
       </c>
       <c r="F1732" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1733" spans="1:6" x14ac:dyDescent="0.3">
@@ -53210,7 +53213,7 @@
         <v>1905</v>
       </c>
       <c r="F1749" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1750" spans="1:6" x14ac:dyDescent="0.3">
@@ -53410,7 +53413,7 @@
         <v>2</v>
       </c>
       <c r="F1759" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1760" spans="1:6" x14ac:dyDescent="0.3">
@@ -53810,7 +53813,7 @@
         <v>1905</v>
       </c>
       <c r="F1779" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1780" spans="1:6" x14ac:dyDescent="0.3">
@@ -54010,7 +54013,7 @@
         <v>2</v>
       </c>
       <c r="F1789" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1790" spans="1:6" x14ac:dyDescent="0.3">
@@ -54110,7 +54113,7 @@
         <v>1905</v>
       </c>
       <c r="F1794" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1795" spans="1:6" x14ac:dyDescent="0.3">
@@ -54310,7 +54313,7 @@
         <v>40</v>
       </c>
       <c r="F1804" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1805" spans="1:6" x14ac:dyDescent="0.3">
@@ -54410,7 +54413,7 @@
         <v>1905</v>
       </c>
       <c r="F1809" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1810" spans="1:6" x14ac:dyDescent="0.3">
@@ -54610,7 +54613,7 @@
         <v>64</v>
       </c>
       <c r="F1819" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1820" spans="1:6" x14ac:dyDescent="0.3">
@@ -54650,7 +54653,7 @@
         <v>1905</v>
       </c>
       <c r="F1821" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1822" spans="1:6" x14ac:dyDescent="0.3">
@@ -54850,7 +54853,7 @@
         <v>6</v>
       </c>
       <c r="F1831" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1832" spans="1:6" x14ac:dyDescent="0.3">
@@ -54890,7 +54893,7 @@
         <v>1905</v>
       </c>
       <c r="F1833" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1834" spans="1:6" x14ac:dyDescent="0.3">
@@ -55090,7 +55093,7 @@
         <v>6</v>
       </c>
       <c r="F1843" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1844" spans="1:6" x14ac:dyDescent="0.3">
@@ -55130,7 +55133,7 @@
         <v>1905</v>
       </c>
       <c r="F1845" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1846" spans="1:6" x14ac:dyDescent="0.3">
@@ -55330,7 +55333,7 @@
         <v>6</v>
       </c>
       <c r="F1855" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1856" spans="1:6" x14ac:dyDescent="0.3">
@@ -55370,7 +55373,7 @@
         <v>1905</v>
       </c>
       <c r="F1857" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1858" spans="1:6" x14ac:dyDescent="0.3">
@@ -55550,7 +55553,7 @@
         <v>1905</v>
       </c>
       <c r="F1866" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1867" spans="1:6" x14ac:dyDescent="0.3">
@@ -55570,7 +55573,7 @@
         <v>6</v>
       </c>
       <c r="F1867" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1868" spans="1:6" x14ac:dyDescent="0.3">
@@ -55730,7 +55733,7 @@
         <v>1905</v>
       </c>
       <c r="F1875" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1876" spans="1:6" x14ac:dyDescent="0.3">
@@ -55750,7 +55753,7 @@
         <v>2</v>
       </c>
       <c r="F1876" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1877" spans="1:6" x14ac:dyDescent="0.3">
@@ -55930,7 +55933,7 @@
         <v>6</v>
       </c>
       <c r="F1885" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1886" spans="1:6" x14ac:dyDescent="0.3">
@@ -55970,7 +55973,7 @@
         <v>1905</v>
       </c>
       <c r="F1887" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1888" spans="1:6" x14ac:dyDescent="0.3">
@@ -56150,7 +56153,7 @@
         <v>1905</v>
       </c>
       <c r="F1896" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1897" spans="1:6" x14ac:dyDescent="0.3">
@@ -56170,7 +56173,7 @@
         <v>69</v>
       </c>
       <c r="F1897" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1898" spans="1:6" x14ac:dyDescent="0.3">
@@ -56350,7 +56353,7 @@
         <v>6</v>
       </c>
       <c r="F1906" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1907" spans="1:6" x14ac:dyDescent="0.3">
@@ -56410,7 +56413,7 @@
         <v>1905</v>
       </c>
       <c r="F1909" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1910" spans="1:6" x14ac:dyDescent="0.3">
@@ -56610,7 +56613,7 @@
         <v>64</v>
       </c>
       <c r="F1919" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1920" spans="1:6" x14ac:dyDescent="0.3">
@@ -56730,7 +56733,7 @@
         <v>1905</v>
       </c>
       <c r="F1925" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1926" spans="1:6" x14ac:dyDescent="0.3">
@@ -56930,7 +56933,7 @@
         <v>64</v>
       </c>
       <c r="F1935" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1936" spans="1:6" x14ac:dyDescent="0.3">
@@ -57270,7 +57273,7 @@
         <v>1905</v>
       </c>
       <c r="F1952" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1953" spans="1:6" x14ac:dyDescent="0.3">
@@ -57470,7 +57473,7 @@
         <v>6</v>
       </c>
       <c r="F1962" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1963" spans="1:6" x14ac:dyDescent="0.3">
@@ -57890,7 +57893,7 @@
         <v>1905</v>
       </c>
       <c r="F1983" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1984" spans="1:6" x14ac:dyDescent="0.3">
@@ -57950,7 +57953,7 @@
         <v>1905</v>
       </c>
       <c r="F1986" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1987" spans="1:6" x14ac:dyDescent="0.3">
@@ -58070,7 +58073,7 @@
         <v>1905</v>
       </c>
       <c r="F1992" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1993" spans="1:6" x14ac:dyDescent="0.3">
@@ -58090,7 +58093,7 @@
         <v>2</v>
       </c>
       <c r="F1993" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1994" spans="1:6" x14ac:dyDescent="0.3">
@@ -58170,7 +58173,7 @@
         <v>1905</v>
       </c>
       <c r="F1997" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1998" spans="1:6" x14ac:dyDescent="0.3">
@@ -58210,7 +58213,7 @@
         <v>40</v>
       </c>
       <c r="F1999" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2000" spans="1:6" x14ac:dyDescent="0.3">
@@ -58230,7 +58233,7 @@
         <v>2</v>
       </c>
       <c r="F2000" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2001" spans="1:6" x14ac:dyDescent="0.3">
@@ -58250,7 +58253,7 @@
         <v>2</v>
       </c>
       <c r="F2001" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2002" spans="1:6" x14ac:dyDescent="0.3">
@@ -58430,7 +58433,7 @@
         <v>1905</v>
       </c>
       <c r="F2010" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2011" spans="1:6" x14ac:dyDescent="0.3">
@@ -58630,7 +58633,7 @@
         <v>2</v>
       </c>
       <c r="F2020" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2021" spans="1:6" x14ac:dyDescent="0.3">
@@ -58910,7 +58913,7 @@
         <v>1905</v>
       </c>
       <c r="F2034" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2035" spans="1:6" x14ac:dyDescent="0.3">
@@ -59110,7 +59113,7 @@
         <v>6</v>
       </c>
       <c r="F2044" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2045" spans="1:6" x14ac:dyDescent="0.3">
@@ -59390,7 +59393,7 @@
         <v>1905</v>
       </c>
       <c r="F2058" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2059" spans="1:6" x14ac:dyDescent="0.3">
@@ -59590,7 +59593,7 @@
         <v>2</v>
       </c>
       <c r="F2068" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2069" spans="1:6" x14ac:dyDescent="0.3">
@@ -59810,7 +59813,7 @@
         <v>1905</v>
       </c>
       <c r="F2079" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2080" spans="1:6" x14ac:dyDescent="0.3">
@@ -60010,7 +60013,7 @@
         <v>6</v>
       </c>
       <c r="F2089" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2090" spans="1:6" x14ac:dyDescent="0.3">
@@ -60350,7 +60353,7 @@
         <v>1905</v>
       </c>
       <c r="F2106" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2107" spans="1:6" x14ac:dyDescent="0.3">
@@ -60550,7 +60553,7 @@
         <v>2</v>
       </c>
       <c r="F2116" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2117" spans="1:6" x14ac:dyDescent="0.3">
@@ -60950,7 +60953,7 @@
         <v>1905</v>
       </c>
       <c r="F2136" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2137" spans="1:6" x14ac:dyDescent="0.3">
@@ -61150,7 +61153,7 @@
         <v>2</v>
       </c>
       <c r="F2146" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2147" spans="1:6" x14ac:dyDescent="0.3">
@@ -61250,7 +61253,7 @@
         <v>1905</v>
       </c>
       <c r="F2151" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2152" spans="1:6" x14ac:dyDescent="0.3">
@@ -61450,7 +61453,7 @@
         <v>40</v>
       </c>
       <c r="F2161" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2162" spans="1:6" x14ac:dyDescent="0.3">
@@ -61550,7 +61553,7 @@
         <v>1905</v>
       </c>
       <c r="F2166" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2167" spans="1:6" x14ac:dyDescent="0.3">
@@ -61750,7 +61753,7 @@
         <v>64</v>
       </c>
       <c r="F2176" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2177" spans="1:6" x14ac:dyDescent="0.3">
@@ -61790,7 +61793,7 @@
         <v>1905</v>
       </c>
       <c r="F2178" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2179" spans="1:6" x14ac:dyDescent="0.3">
@@ -61990,7 +61993,7 @@
         <v>6</v>
       </c>
       <c r="F2188" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2189" spans="1:6" x14ac:dyDescent="0.3">
@@ -62030,7 +62033,7 @@
         <v>1905</v>
       </c>
       <c r="F2190" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2191" spans="1:6" x14ac:dyDescent="0.3">
@@ -62230,7 +62233,7 @@
         <v>6</v>
       </c>
       <c r="F2200" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2201" spans="1:6" x14ac:dyDescent="0.3">
@@ -62270,7 +62273,7 @@
         <v>1905</v>
       </c>
       <c r="F2202" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2203" spans="1:6" x14ac:dyDescent="0.3">
@@ -62470,7 +62473,7 @@
         <v>6</v>
       </c>
       <c r="F2212" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2213" spans="1:6" x14ac:dyDescent="0.3">
@@ -62510,7 +62513,7 @@
         <v>1905</v>
       </c>
       <c r="F2214" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2215" spans="1:6" x14ac:dyDescent="0.3">
@@ -62690,7 +62693,7 @@
         <v>1905</v>
       </c>
       <c r="F2223" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2224" spans="1:6" x14ac:dyDescent="0.3">
@@ -62710,7 +62713,7 @@
         <v>6</v>
       </c>
       <c r="F2224" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2225" spans="1:6" x14ac:dyDescent="0.3">
@@ -62870,7 +62873,7 @@
         <v>1905</v>
       </c>
       <c r="F2232" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2233" spans="1:6" x14ac:dyDescent="0.3">
@@ -62890,7 +62893,7 @@
         <v>2</v>
       </c>
       <c r="F2233" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2234" spans="1:6" x14ac:dyDescent="0.3">
@@ -63070,7 +63073,7 @@
         <v>6</v>
       </c>
       <c r="F2242" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2243" spans="1:6" x14ac:dyDescent="0.3">
@@ -63110,7 +63113,7 @@
         <v>1905</v>
       </c>
       <c r="F2244" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2245" spans="1:6" x14ac:dyDescent="0.3">
@@ -63290,7 +63293,7 @@
         <v>1905</v>
       </c>
       <c r="F2253" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2254" spans="1:6" x14ac:dyDescent="0.3">
@@ -63310,7 +63313,7 @@
         <v>69</v>
       </c>
       <c r="F2254" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2255" spans="1:6" x14ac:dyDescent="0.3">
@@ -63490,7 +63493,7 @@
         <v>6</v>
       </c>
       <c r="F2263" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2264" spans="1:6" x14ac:dyDescent="0.3">
@@ -63550,7 +63553,7 @@
         <v>1905</v>
       </c>
       <c r="F2266" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2267" spans="1:6" x14ac:dyDescent="0.3">
@@ -63750,7 +63753,7 @@
         <v>64</v>
       </c>
       <c r="F2276" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2277" spans="1:6" x14ac:dyDescent="0.3">
@@ -63870,7 +63873,7 @@
         <v>1905</v>
       </c>
       <c r="F2282" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2283" spans="1:6" x14ac:dyDescent="0.3">
@@ -64070,7 +64073,7 @@
         <v>64</v>
       </c>
       <c r="F2292" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2293" spans="1:6" x14ac:dyDescent="0.3">
@@ -64410,7 +64413,7 @@
         <v>1905</v>
       </c>
       <c r="F2309" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2310" spans="1:6" x14ac:dyDescent="0.3">
@@ -64610,7 +64613,7 @@
         <v>6</v>
       </c>
       <c r="F2319" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2320" spans="1:6" x14ac:dyDescent="0.3">
@@ -65030,7 +65033,7 @@
         <v>1905</v>
       </c>
       <c r="F2340" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2341" spans="1:6" x14ac:dyDescent="0.3">
@@ -65090,7 +65093,7 @@
         <v>1905</v>
       </c>
       <c r="F2343" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2344" spans="1:6" x14ac:dyDescent="0.3">
@@ -65210,7 +65213,7 @@
         <v>1905</v>
       </c>
       <c r="F2349" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2350" spans="1:6" x14ac:dyDescent="0.3">
@@ -65230,7 +65233,7 @@
         <v>2</v>
       </c>
       <c r="F2350" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2351" spans="1:6" x14ac:dyDescent="0.3">
@@ -65310,7 +65313,7 @@
         <v>1905</v>
       </c>
       <c r="F2354" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2355" spans="1:6" x14ac:dyDescent="0.3">
@@ -65350,7 +65353,7 @@
         <v>40</v>
       </c>
       <c r="F2356" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2357" spans="1:6" x14ac:dyDescent="0.3">
@@ -65370,7 +65373,7 @@
         <v>2</v>
       </c>
       <c r="F2357" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2358" spans="1:6" x14ac:dyDescent="0.3">
@@ -65390,7 +65393,7 @@
         <v>2</v>
       </c>
       <c r="F2358" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2359" spans="1:6" x14ac:dyDescent="0.3">
@@ -65430,7 +65433,7 @@
         <v>1905</v>
       </c>
       <c r="F2360" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2361" spans="1:6" x14ac:dyDescent="0.3">
@@ -65510,7 +65513,7 @@
         <v>6</v>
       </c>
       <c r="F2364" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2365" spans="1:6" x14ac:dyDescent="0.3">
@@ -65630,7 +65633,7 @@
         <v>2</v>
       </c>
       <c r="F2370" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2371" spans="1:6" x14ac:dyDescent="0.3">
@@ -65950,7 +65953,7 @@
         <v>1905</v>
       </c>
       <c r="F2386" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2387" spans="1:6" x14ac:dyDescent="0.3">
@@ -66150,7 +66153,7 @@
         <v>2</v>
       </c>
       <c r="F2396" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2397" spans="1:6" x14ac:dyDescent="0.3">
@@ -66370,7 +66373,7 @@
         <v>1905</v>
       </c>
       <c r="F2407" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2408" spans="1:6" x14ac:dyDescent="0.3">
@@ -66570,7 +66573,7 @@
         <v>2</v>
       </c>
       <c r="F2417" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2418" spans="1:6" x14ac:dyDescent="0.3">
@@ -66850,7 +66853,7 @@
         <v>1905</v>
       </c>
       <c r="F2431" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2432" spans="1:6" x14ac:dyDescent="0.3">
@@ -67050,7 +67053,7 @@
         <v>2</v>
       </c>
       <c r="F2441" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2442" spans="1:6" x14ac:dyDescent="0.3">
@@ -67290,7 +67293,7 @@
         <v>1905</v>
       </c>
       <c r="F2453" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2454" spans="1:6" x14ac:dyDescent="0.3">
@@ -67490,7 +67493,7 @@
         <v>6</v>
       </c>
       <c r="F2463" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2464" spans="1:6" x14ac:dyDescent="0.3">
@@ -67710,7 +67713,7 @@
         <v>1905</v>
       </c>
       <c r="F2474" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2475" spans="1:6" x14ac:dyDescent="0.3">
@@ -67910,7 +67913,7 @@
         <v>2</v>
       </c>
       <c r="F2484" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2485" spans="1:6" x14ac:dyDescent="0.3">
@@ -68190,7 +68193,7 @@
         <v>1905</v>
       </c>
       <c r="F2498" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2499" spans="1:6" x14ac:dyDescent="0.3">
@@ -68390,7 +68393,7 @@
         <v>2</v>
       </c>
       <c r="F2508" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2509" spans="1:6" x14ac:dyDescent="0.3">
@@ -68490,7 +68493,7 @@
         <v>1905</v>
       </c>
       <c r="F2513" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2514" spans="1:6" x14ac:dyDescent="0.3">
@@ -68690,7 +68693,7 @@
         <v>2</v>
       </c>
       <c r="F2523" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2524" spans="1:6" x14ac:dyDescent="0.3">
@@ -69030,7 +69033,7 @@
         <v>1905</v>
       </c>
       <c r="F2540" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2541" spans="1:6" x14ac:dyDescent="0.3">
@@ -69230,7 +69233,7 @@
         <v>2</v>
       </c>
       <c r="F2550" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2551" spans="1:6" x14ac:dyDescent="0.3">
@@ -69510,7 +69513,7 @@
         <v>1905</v>
       </c>
       <c r="F2564" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2565" spans="1:6" x14ac:dyDescent="0.3">
@@ -69710,7 +69713,7 @@
         <v>6</v>
       </c>
       <c r="F2574" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2575" spans="1:6" x14ac:dyDescent="0.3">
@@ -69930,7 +69933,7 @@
         <v>1905</v>
       </c>
       <c r="F2585" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2586" spans="1:6" x14ac:dyDescent="0.3">
@@ -70130,7 +70133,7 @@
         <v>6</v>
       </c>
       <c r="F2595" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2596" spans="1:6" x14ac:dyDescent="0.3">
@@ -70170,7 +70173,7 @@
         <v>1905</v>
       </c>
       <c r="F2597" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2598" spans="1:6" x14ac:dyDescent="0.3">
@@ -70370,7 +70373,7 @@
         <v>2</v>
       </c>
       <c r="F2607" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2608" spans="1:6" x14ac:dyDescent="0.3">
@@ -70410,7 +70413,7 @@
         <v>1905</v>
       </c>
       <c r="F2609" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2610" spans="1:6" x14ac:dyDescent="0.3">
@@ -70590,7 +70593,7 @@
         <v>1905</v>
       </c>
       <c r="F2618" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2619" spans="1:6" x14ac:dyDescent="0.3">
@@ -70610,7 +70613,7 @@
         <v>2</v>
       </c>
       <c r="F2619" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2620" spans="1:6" x14ac:dyDescent="0.3">
@@ -70790,7 +70793,7 @@
         <v>2</v>
       </c>
       <c r="F2628" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2629" spans="1:6" x14ac:dyDescent="0.3">
@@ -70830,7 +70833,7 @@
         <v>1905</v>
       </c>
       <c r="F2630" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2631" spans="1:6" x14ac:dyDescent="0.3">
@@ -71030,7 +71033,7 @@
         <v>2</v>
       </c>
       <c r="F2640" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2641" spans="1:6" x14ac:dyDescent="0.3">
@@ -71070,7 +71073,7 @@
         <v>1905</v>
       </c>
       <c r="F2642" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2643" spans="1:6" x14ac:dyDescent="0.3">
@@ -71270,7 +71273,7 @@
         <v>2</v>
       </c>
       <c r="F2652" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2653" spans="1:6" x14ac:dyDescent="0.3">
@@ -71310,7 +71313,7 @@
         <v>1905</v>
       </c>
       <c r="F2654" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2655" spans="1:6" x14ac:dyDescent="0.3">
@@ -71510,7 +71513,7 @@
         <v>6</v>
       </c>
       <c r="F2664" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2665" spans="1:6" x14ac:dyDescent="0.3">
@@ -71610,7 +71613,7 @@
         <v>1905</v>
       </c>
       <c r="F2669" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2670" spans="1:6" x14ac:dyDescent="0.3">
@@ -71810,7 +71813,7 @@
         <v>6</v>
       </c>
       <c r="F2679" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2680" spans="1:6" x14ac:dyDescent="0.3">
@@ -71850,7 +71853,7 @@
         <v>1905</v>
       </c>
       <c r="F2681" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2682" spans="1:6" x14ac:dyDescent="0.3">
@@ -72030,7 +72033,7 @@
         <v>1905</v>
       </c>
       <c r="F2690" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2691" spans="1:6" x14ac:dyDescent="0.3">
@@ -72050,7 +72053,7 @@
         <v>64</v>
       </c>
       <c r="F2691" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2692" spans="1:6" x14ac:dyDescent="0.3">
@@ -72230,7 +72233,7 @@
         <v>6</v>
       </c>
       <c r="F2700" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2701" spans="1:6" x14ac:dyDescent="0.3">
@@ -72390,7 +72393,7 @@
         <v>1905</v>
       </c>
       <c r="F2708" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2709" spans="1:6" x14ac:dyDescent="0.3">
@@ -72570,7 +72573,7 @@
         <v>1905</v>
       </c>
       <c r="F2717" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2718" spans="1:6" x14ac:dyDescent="0.3">
@@ -72590,7 +72593,7 @@
         <v>2</v>
       </c>
       <c r="F2718" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2719" spans="1:6" x14ac:dyDescent="0.3">
@@ -72770,7 +72773,7 @@
         <v>40</v>
       </c>
       <c r="F2727" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2728" spans="1:6" x14ac:dyDescent="0.3">
@@ -72810,7 +72813,7 @@
         <v>1905</v>
       </c>
       <c r="F2729" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2730" spans="1:6" x14ac:dyDescent="0.3">
@@ -73010,7 +73013,7 @@
         <v>6</v>
       </c>
       <c r="F2739" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2740" spans="1:6" x14ac:dyDescent="0.3">
@@ -73110,7 +73113,7 @@
         <v>1905</v>
       </c>
       <c r="F2744" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2745" spans="1:6" x14ac:dyDescent="0.3">
@@ -73310,7 +73313,7 @@
         <v>64</v>
       </c>
       <c r="F2754" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2755" spans="1:6" x14ac:dyDescent="0.3">
@@ -73350,7 +73353,7 @@
         <v>1905</v>
       </c>
       <c r="F2756" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2757" spans="1:6" x14ac:dyDescent="0.3">
@@ -73550,7 +73553,7 @@
         <v>2</v>
       </c>
       <c r="F2766" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2767" spans="1:6" x14ac:dyDescent="0.3">
@@ -73590,7 +73593,7 @@
         <v>1905</v>
       </c>
       <c r="F2768" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2769" spans="1:6" x14ac:dyDescent="0.3">
@@ -73770,7 +73773,7 @@
         <v>1905</v>
       </c>
       <c r="F2777" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2778" spans="1:6" x14ac:dyDescent="0.3">
@@ -73790,7 +73793,7 @@
         <v>64</v>
       </c>
       <c r="F2778" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2779" spans="1:6" x14ac:dyDescent="0.3">
@@ -73970,7 +73973,7 @@
         <v>2</v>
       </c>
       <c r="F2787" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2788" spans="1:6" x14ac:dyDescent="0.3">
@@ -74070,7 +74073,7 @@
         <v>1905</v>
       </c>
       <c r="F2792" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2793" spans="1:6" x14ac:dyDescent="0.3">
@@ -74270,7 +74273,7 @@
         <v>2</v>
       </c>
       <c r="F2802" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2803" spans="1:6" x14ac:dyDescent="0.3">
@@ -74370,7 +74373,7 @@
         <v>1905</v>
       </c>
       <c r="F2807" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2808" spans="1:6" x14ac:dyDescent="0.3">
@@ -74570,7 +74573,7 @@
         <v>2</v>
       </c>
       <c r="F2817" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2818" spans="1:6" x14ac:dyDescent="0.3">
@@ -74730,7 +74733,7 @@
         <v>1905</v>
       </c>
       <c r="F2825" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2826" spans="1:6" x14ac:dyDescent="0.3">
@@ -74930,7 +74933,7 @@
         <v>6</v>
       </c>
       <c r="F2835" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2836" spans="1:6" x14ac:dyDescent="0.3">
@@ -75030,7 +75033,7 @@
         <v>1905</v>
       </c>
       <c r="F2840" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2841" spans="1:6" x14ac:dyDescent="0.3">
@@ -75230,7 +75233,7 @@
         <v>2</v>
       </c>
       <c r="F2850" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2851" spans="1:6" x14ac:dyDescent="0.3">
@@ -75390,7 +75393,7 @@
         <v>1905</v>
       </c>
       <c r="F2858" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2859" spans="1:6" x14ac:dyDescent="0.3">
@@ -75590,7 +75593,7 @@
         <v>2</v>
       </c>
       <c r="F2868" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2869" spans="1:6" x14ac:dyDescent="0.3">
@@ -75750,7 +75753,7 @@
         <v>1905</v>
       </c>
       <c r="F2876" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2877" spans="1:6" x14ac:dyDescent="0.3">
@@ -75950,7 +75953,7 @@
         <v>2</v>
       </c>
       <c r="F2886" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2887" spans="1:6" x14ac:dyDescent="0.3">
@@ -76110,7 +76113,7 @@
         <v>1905</v>
       </c>
       <c r="F2894" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2895" spans="1:6" x14ac:dyDescent="0.3">
@@ -76310,7 +76313,7 @@
         <v>6</v>
       </c>
       <c r="F2904" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2905" spans="1:6" x14ac:dyDescent="0.3">
@@ -76410,7 +76413,7 @@
         <v>1905</v>
       </c>
       <c r="F2909" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2910" spans="1:6" x14ac:dyDescent="0.3">
@@ -76610,7 +76613,7 @@
         <v>2</v>
       </c>
       <c r="F2919" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2920" spans="1:6" x14ac:dyDescent="0.3">
@@ -76890,7 +76893,7 @@
         <v>1905</v>
       </c>
       <c r="F2933" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2934" spans="1:6" x14ac:dyDescent="0.3">
@@ -77090,7 +77093,7 @@
         <v>6</v>
       </c>
       <c r="F2943" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2944" spans="1:6" x14ac:dyDescent="0.3">
@@ -77250,7 +77253,7 @@
         <v>1905</v>
       </c>
       <c r="F2951" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2952" spans="1:6" x14ac:dyDescent="0.3">
@@ -77450,7 +77453,7 @@
         <v>64</v>
       </c>
       <c r="F2961" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2962" spans="1:6" x14ac:dyDescent="0.3">
@@ -77610,7 +77613,7 @@
         <v>1905</v>
       </c>
       <c r="F2969" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2970" spans="1:6" x14ac:dyDescent="0.3">
@@ -77810,7 +77813,7 @@
         <v>6</v>
       </c>
       <c r="F2979" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2980" spans="1:6" x14ac:dyDescent="0.3">
@@ -77970,7 +77973,7 @@
         <v>1905</v>
       </c>
       <c r="F2987" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2988" spans="1:6" x14ac:dyDescent="0.3">
@@ -78170,7 +78173,7 @@
         <v>6</v>
       </c>
       <c r="F2997" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2998" spans="1:6" x14ac:dyDescent="0.3">
@@ -78330,7 +78333,7 @@
         <v>6</v>
       </c>
       <c r="F3005" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3006" spans="1:6" x14ac:dyDescent="0.3">
@@ -78450,7 +78453,7 @@
         <v>2</v>
       </c>
       <c r="F3011" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3012" spans="1:6" x14ac:dyDescent="0.3">
@@ -78770,7 +78773,7 @@
         <v>1905</v>
       </c>
       <c r="F3027" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3028" spans="1:6" x14ac:dyDescent="0.3">
@@ -78970,7 +78973,7 @@
         <v>2</v>
       </c>
       <c r="F3037" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3038" spans="1:6" x14ac:dyDescent="0.3">
@@ -79190,7 +79193,7 @@
         <v>1905</v>
       </c>
       <c r="F3048" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3049" spans="1:6" x14ac:dyDescent="0.3">
@@ -79390,7 +79393,7 @@
         <v>2</v>
       </c>
       <c r="F3058" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3059" spans="1:6" x14ac:dyDescent="0.3">
@@ -79670,7 +79673,7 @@
         <v>1905</v>
       </c>
       <c r="F3072" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3073" spans="1:6" x14ac:dyDescent="0.3">
@@ -79870,7 +79873,7 @@
         <v>2</v>
       </c>
       <c r="F3082" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3083" spans="1:6" x14ac:dyDescent="0.3">
@@ -80110,7 +80113,7 @@
         <v>1905</v>
       </c>
       <c r="F3094" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3095" spans="1:6" x14ac:dyDescent="0.3">
@@ -80310,7 +80313,7 @@
         <v>6</v>
       </c>
       <c r="F3104" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3105" spans="1:6" x14ac:dyDescent="0.3">
@@ -80530,7 +80533,7 @@
         <v>1905</v>
       </c>
       <c r="F3115" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3116" spans="1:6" x14ac:dyDescent="0.3">
@@ -80730,7 +80733,7 @@
         <v>2</v>
       </c>
       <c r="F3125" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3126" spans="1:6" x14ac:dyDescent="0.3">
@@ -81010,7 +81013,7 @@
         <v>1905</v>
       </c>
       <c r="F3139" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3140" spans="1:6" x14ac:dyDescent="0.3">
@@ -81210,7 +81213,7 @@
         <v>2</v>
       </c>
       <c r="F3149" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3150" spans="1:6" x14ac:dyDescent="0.3">
@@ -81310,7 +81313,7 @@
         <v>1905</v>
       </c>
       <c r="F3154" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3155" spans="1:6" x14ac:dyDescent="0.3">
@@ -81510,7 +81513,7 @@
         <v>2</v>
       </c>
       <c r="F3164" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3165" spans="1:6" x14ac:dyDescent="0.3">
@@ -81850,7 +81853,7 @@
         <v>1905</v>
       </c>
       <c r="F3181" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3182" spans="1:6" x14ac:dyDescent="0.3">
@@ -82050,7 +82053,7 @@
         <v>2</v>
       </c>
       <c r="F3191" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3192" spans="1:6" x14ac:dyDescent="0.3">
@@ -82330,7 +82333,7 @@
         <v>1905</v>
       </c>
       <c r="F3205" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3206" spans="1:6" x14ac:dyDescent="0.3">
@@ -82530,7 +82533,7 @@
         <v>6</v>
       </c>
       <c r="F3215" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3216" spans="1:6" x14ac:dyDescent="0.3">
@@ -82750,7 +82753,7 @@
         <v>1905</v>
       </c>
       <c r="F3226" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3227" spans="1:6" x14ac:dyDescent="0.3">
@@ -82950,7 +82953,7 @@
         <v>6</v>
       </c>
       <c r="F3236" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3237" spans="1:6" x14ac:dyDescent="0.3">
@@ -82990,7 +82993,7 @@
         <v>1905</v>
       </c>
       <c r="F3238" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3239" spans="1:6" x14ac:dyDescent="0.3">
@@ -83190,7 +83193,7 @@
         <v>2</v>
       </c>
       <c r="F3248" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3249" spans="1:6" x14ac:dyDescent="0.3">
@@ -83230,7 +83233,7 @@
         <v>1905</v>
       </c>
       <c r="F3250" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3251" spans="1:6" x14ac:dyDescent="0.3">
@@ -83410,7 +83413,7 @@
         <v>1905</v>
       </c>
       <c r="F3259" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3260" spans="1:6" x14ac:dyDescent="0.3">
@@ -83430,7 +83433,7 @@
         <v>2</v>
       </c>
       <c r="F3260" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3261" spans="1:6" x14ac:dyDescent="0.3">
@@ -83610,7 +83613,7 @@
         <v>2</v>
       </c>
       <c r="F3269" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3270" spans="1:6" x14ac:dyDescent="0.3">
@@ -83650,7 +83653,7 @@
         <v>1905</v>
       </c>
       <c r="F3271" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3272" spans="1:6" x14ac:dyDescent="0.3">
@@ -83850,7 +83853,7 @@
         <v>2</v>
       </c>
       <c r="F3281" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3282" spans="1:6" x14ac:dyDescent="0.3">
@@ -83890,7 +83893,7 @@
         <v>1905</v>
       </c>
       <c r="F3283" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3284" spans="1:6" x14ac:dyDescent="0.3">
@@ -84090,7 +84093,7 @@
         <v>2</v>
       </c>
       <c r="F3293" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3294" spans="1:6" x14ac:dyDescent="0.3">
@@ -84130,7 +84133,7 @@
         <v>1905</v>
       </c>
       <c r="F3295" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3296" spans="1:6" x14ac:dyDescent="0.3">
@@ -84330,7 +84333,7 @@
         <v>6</v>
       </c>
       <c r="F3305" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3306" spans="1:6" x14ac:dyDescent="0.3">
@@ -84430,7 +84433,7 @@
         <v>1905</v>
       </c>
       <c r="F3310" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3311" spans="1:6" x14ac:dyDescent="0.3">
@@ -84630,7 +84633,7 @@
         <v>6</v>
       </c>
       <c r="F3320" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3321" spans="1:6" x14ac:dyDescent="0.3">
@@ -84670,7 +84673,7 @@
         <v>1905</v>
       </c>
       <c r="F3322" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3323" spans="1:6" x14ac:dyDescent="0.3">
@@ -84850,7 +84853,7 @@
         <v>1905</v>
       </c>
       <c r="F3331" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3332" spans="1:6" x14ac:dyDescent="0.3">
@@ -84870,7 +84873,7 @@
         <v>64</v>
       </c>
       <c r="F3332" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3333" spans="1:6" x14ac:dyDescent="0.3">
@@ -85050,7 +85053,7 @@
         <v>6</v>
       </c>
       <c r="F3341" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3342" spans="1:6" x14ac:dyDescent="0.3">
@@ -85210,7 +85213,7 @@
         <v>1905</v>
       </c>
       <c r="F3349" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3350" spans="1:6" x14ac:dyDescent="0.3">
@@ -85390,7 +85393,7 @@
         <v>1905</v>
       </c>
       <c r="F3358" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3359" spans="1:6" x14ac:dyDescent="0.3">
@@ -85410,7 +85413,7 @@
         <v>2</v>
       </c>
       <c r="F3359" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3360" spans="1:6" x14ac:dyDescent="0.3">
@@ -85590,7 +85593,7 @@
         <v>40</v>
       </c>
       <c r="F3368" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3369" spans="1:6" x14ac:dyDescent="0.3">
@@ -85630,7 +85633,7 @@
         <v>1905</v>
       </c>
       <c r="F3370" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3371" spans="1:6" x14ac:dyDescent="0.3">
@@ -85830,7 +85833,7 @@
         <v>6</v>
       </c>
       <c r="F3380" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3381" spans="1:6" x14ac:dyDescent="0.3">
@@ -85930,7 +85933,7 @@
         <v>1905</v>
       </c>
       <c r="F3385" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3386" spans="1:6" x14ac:dyDescent="0.3">
@@ -86130,7 +86133,7 @@
         <v>64</v>
       </c>
       <c r="F3395" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3396" spans="1:6" x14ac:dyDescent="0.3">
@@ -86170,7 +86173,7 @@
         <v>1905</v>
       </c>
       <c r="F3397" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3398" spans="1:6" x14ac:dyDescent="0.3">
@@ -86370,7 +86373,7 @@
         <v>2</v>
       </c>
       <c r="F3407" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3408" spans="1:6" x14ac:dyDescent="0.3">
@@ -86410,7 +86413,7 @@
         <v>1905</v>
       </c>
       <c r="F3409" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3410" spans="1:6" x14ac:dyDescent="0.3">
@@ -86590,7 +86593,7 @@
         <v>1905</v>
       </c>
       <c r="F3418" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3419" spans="1:6" x14ac:dyDescent="0.3">
@@ -86610,7 +86613,7 @@
         <v>64</v>
       </c>
       <c r="F3419" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3420" spans="1:6" x14ac:dyDescent="0.3">
@@ -86790,7 +86793,7 @@
         <v>2</v>
       </c>
       <c r="F3428" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3429" spans="1:6" x14ac:dyDescent="0.3">
@@ -86890,7 +86893,7 @@
         <v>1905</v>
       </c>
       <c r="F3433" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3434" spans="1:6" x14ac:dyDescent="0.3">
@@ -87090,7 +87093,7 @@
         <v>2</v>
       </c>
       <c r="F3443" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3444" spans="1:6" x14ac:dyDescent="0.3">
@@ -87190,7 +87193,7 @@
         <v>1905</v>
       </c>
       <c r="F3448" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3449" spans="1:6" x14ac:dyDescent="0.3">
@@ -87390,7 +87393,7 @@
         <v>2</v>
       </c>
       <c r="F3458" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3459" spans="1:6" x14ac:dyDescent="0.3">
@@ -87550,7 +87553,7 @@
         <v>1905</v>
       </c>
       <c r="F3466" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3467" spans="1:6" x14ac:dyDescent="0.3">
@@ -87750,7 +87753,7 @@
         <v>6</v>
       </c>
       <c r="F3476" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3477" spans="1:6" x14ac:dyDescent="0.3">
@@ -87850,7 +87853,7 @@
         <v>1905</v>
       </c>
       <c r="F3481" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3482" spans="1:6" x14ac:dyDescent="0.3">
@@ -88050,7 +88053,7 @@
         <v>2</v>
       </c>
       <c r="F3491" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3492" spans="1:6" x14ac:dyDescent="0.3">
@@ -88210,7 +88213,7 @@
         <v>1905</v>
       </c>
       <c r="F3499" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3500" spans="1:6" x14ac:dyDescent="0.3">
@@ -88410,7 +88413,7 @@
         <v>2</v>
       </c>
       <c r="F3509" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3510" spans="1:6" x14ac:dyDescent="0.3">
@@ -88570,7 +88573,7 @@
         <v>1905</v>
       </c>
       <c r="F3517" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3518" spans="1:6" x14ac:dyDescent="0.3">
@@ -88770,7 +88773,7 @@
         <v>2</v>
       </c>
       <c r="F3527" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3528" spans="1:6" x14ac:dyDescent="0.3">
@@ -88930,7 +88933,7 @@
         <v>1905</v>
       </c>
       <c r="F3535" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3536" spans="1:6" x14ac:dyDescent="0.3">
@@ -89130,7 +89133,7 @@
         <v>6</v>
       </c>
       <c r="F3545" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3546" spans="1:6" x14ac:dyDescent="0.3">
@@ -89230,7 +89233,7 @@
         <v>1905</v>
       </c>
       <c r="F3550" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3551" spans="1:6" x14ac:dyDescent="0.3">
@@ -89430,7 +89433,7 @@
         <v>2</v>
       </c>
       <c r="F3560" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3561" spans="1:6" x14ac:dyDescent="0.3">
@@ -89710,7 +89713,7 @@
         <v>1905</v>
       </c>
       <c r="F3574" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3575" spans="1:6" x14ac:dyDescent="0.3">
@@ -89910,7 +89913,7 @@
         <v>6</v>
       </c>
       <c r="F3584" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3585" spans="1:6" x14ac:dyDescent="0.3">
@@ -90070,7 +90073,7 @@
         <v>1905</v>
       </c>
       <c r="F3592" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3593" spans="1:6" x14ac:dyDescent="0.3">
@@ -90270,7 +90273,7 @@
         <v>64</v>
       </c>
       <c r="F3602" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3603" spans="1:6" x14ac:dyDescent="0.3">
@@ -90430,7 +90433,7 @@
         <v>1905</v>
       </c>
       <c r="F3610" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3611" spans="1:6" x14ac:dyDescent="0.3">
@@ -90630,7 +90633,7 @@
         <v>6</v>
       </c>
       <c r="F3620" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3621" spans="1:6" x14ac:dyDescent="0.3">
@@ -90790,7 +90793,7 @@
         <v>1905</v>
       </c>
       <c r="F3628" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3629" spans="1:6" x14ac:dyDescent="0.3">
@@ -90990,7 +90993,7 @@
         <v>6</v>
       </c>
       <c r="F3638" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3639" spans="1:6" x14ac:dyDescent="0.3">
@@ -91270,7 +91273,7 @@
         <v>1905</v>
       </c>
       <c r="F3652" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3653" spans="1:6" x14ac:dyDescent="0.3">
@@ -91470,7 +91473,7 @@
         <v>2</v>
       </c>
       <c r="F3662" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3663" spans="1:6" x14ac:dyDescent="0.3">
@@ -91750,7 +91753,7 @@
         <v>1905</v>
       </c>
       <c r="F3676" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3677" spans="1:6" x14ac:dyDescent="0.3">
@@ -91950,7 +91953,7 @@
         <v>6</v>
       </c>
       <c r="F3686" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3687" spans="1:6" x14ac:dyDescent="0.3">
@@ -92230,7 +92233,7 @@
         <v>1905</v>
       </c>
       <c r="F3700" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3701" spans="1:6" x14ac:dyDescent="0.3">
@@ -92430,7 +92433,7 @@
         <v>2</v>
       </c>
       <c r="F3710" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3711" spans="1:6" x14ac:dyDescent="0.3">
@@ -92650,7 +92653,7 @@
         <v>1905</v>
       </c>
       <c r="F3721" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3722" spans="1:6" x14ac:dyDescent="0.3">
@@ -92850,7 +92853,7 @@
         <v>6</v>
       </c>
       <c r="F3731" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3732" spans="1:6" x14ac:dyDescent="0.3">
@@ -93190,7 +93193,7 @@
         <v>1905</v>
       </c>
       <c r="F3748" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3749" spans="1:6" x14ac:dyDescent="0.3">
@@ -93390,7 +93393,7 @@
         <v>2</v>
       </c>
       <c r="F3758" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3759" spans="1:6" x14ac:dyDescent="0.3">
@@ -93790,7 +93793,7 @@
         <v>1905</v>
       </c>
       <c r="F3778" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3779" spans="1:6" x14ac:dyDescent="0.3">
@@ -93990,7 +93993,7 @@
         <v>2</v>
       </c>
       <c r="F3788" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3789" spans="1:6" x14ac:dyDescent="0.3">
@@ -94090,7 +94093,7 @@
         <v>1905</v>
       </c>
       <c r="F3793" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3794" spans="1:6" x14ac:dyDescent="0.3">
@@ -94290,7 +94293,7 @@
         <v>40</v>
       </c>
       <c r="F3803" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3804" spans="1:6" x14ac:dyDescent="0.3">
@@ -94390,7 +94393,7 @@
         <v>1905</v>
       </c>
       <c r="F3808" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3809" spans="1:6" x14ac:dyDescent="0.3">
@@ -94590,7 +94593,7 @@
         <v>64</v>
       </c>
       <c r="F3818" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3819" spans="1:6" x14ac:dyDescent="0.3">
@@ -94630,7 +94633,7 @@
         <v>1905</v>
       </c>
       <c r="F3820" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3821" spans="1:6" x14ac:dyDescent="0.3">
@@ -94830,7 +94833,7 @@
         <v>6</v>
       </c>
       <c r="F3830" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3831" spans="1:6" x14ac:dyDescent="0.3">
@@ -94870,7 +94873,7 @@
         <v>1905</v>
       </c>
       <c r="F3832" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3833" spans="1:6" x14ac:dyDescent="0.3">
@@ -95070,7 +95073,7 @@
         <v>6</v>
       </c>
       <c r="F3842" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3843" spans="1:6" x14ac:dyDescent="0.3">
@@ -95110,7 +95113,7 @@
         <v>1905</v>
       </c>
       <c r="F3844" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3845" spans="1:6" x14ac:dyDescent="0.3">
@@ -95310,7 +95313,7 @@
         <v>6</v>
       </c>
       <c r="F3854" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3855" spans="1:6" x14ac:dyDescent="0.3">
@@ -95350,7 +95353,7 @@
         <v>1905</v>
       </c>
       <c r="F3856" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3857" spans="1:6" x14ac:dyDescent="0.3">
@@ -95530,7 +95533,7 @@
         <v>1905</v>
       </c>
       <c r="F3865" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3866" spans="1:6" x14ac:dyDescent="0.3">
@@ -95550,7 +95553,7 @@
         <v>6</v>
       </c>
       <c r="F3866" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3867" spans="1:6" x14ac:dyDescent="0.3">
@@ -95710,7 +95713,7 @@
         <v>1905</v>
       </c>
       <c r="F3874" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3875" spans="1:6" x14ac:dyDescent="0.3">
@@ -95730,7 +95733,7 @@
         <v>2</v>
       </c>
       <c r="F3875" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3876" spans="1:6" x14ac:dyDescent="0.3">
@@ -95910,7 +95913,7 @@
         <v>6</v>
       </c>
       <c r="F3884" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3885" spans="1:6" x14ac:dyDescent="0.3">
@@ -95950,7 +95953,7 @@
         <v>1905</v>
       </c>
       <c r="F3886" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3887" spans="1:6" x14ac:dyDescent="0.3">
@@ -96130,7 +96133,7 @@
         <v>1905</v>
       </c>
       <c r="F3895" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3896" spans="1:6" x14ac:dyDescent="0.3">
@@ -96150,7 +96153,7 @@
         <v>69</v>
       </c>
       <c r="F3896" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3897" spans="1:6" x14ac:dyDescent="0.3">
@@ -96330,7 +96333,7 @@
         <v>6</v>
       </c>
       <c r="F3905" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3906" spans="1:6" x14ac:dyDescent="0.3">
@@ -96390,7 +96393,7 @@
         <v>1905</v>
       </c>
       <c r="F3908" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3909" spans="1:6" x14ac:dyDescent="0.3">
@@ -96590,7 +96593,7 @@
         <v>64</v>
       </c>
       <c r="F3918" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3919" spans="1:6" x14ac:dyDescent="0.3">
@@ -96710,7 +96713,7 @@
         <v>1905</v>
       </c>
       <c r="F3924" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3925" spans="1:6" x14ac:dyDescent="0.3">
@@ -96910,7 +96913,7 @@
         <v>64</v>
       </c>
       <c r="F3934" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3935" spans="1:6" x14ac:dyDescent="0.3">
@@ -97250,7 +97253,7 @@
         <v>1905</v>
       </c>
       <c r="F3951" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3952" spans="1:6" x14ac:dyDescent="0.3">
@@ -97450,7 +97453,7 @@
         <v>6</v>
       </c>
       <c r="F3961" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3962" spans="1:6" x14ac:dyDescent="0.3">
@@ -97870,7 +97873,7 @@
         <v>1905</v>
       </c>
       <c r="F3982" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3983" spans="1:6" x14ac:dyDescent="0.3">
@@ -97930,7 +97933,7 @@
         <v>1905</v>
       </c>
       <c r="F3985" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3986" spans="1:6" x14ac:dyDescent="0.3">
@@ -98050,7 +98053,7 @@
         <v>1905</v>
       </c>
       <c r="F3991" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3992" spans="1:6" x14ac:dyDescent="0.3">
@@ -98070,7 +98073,7 @@
         <v>2</v>
       </c>
       <c r="F3992" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3993" spans="1:6" x14ac:dyDescent="0.3">
@@ -98150,7 +98153,7 @@
         <v>1905</v>
       </c>
       <c r="F3996" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3997" spans="1:6" x14ac:dyDescent="0.3">
@@ -98190,7 +98193,7 @@
         <v>40</v>
       </c>
       <c r="F3998" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3999" spans="1:6" x14ac:dyDescent="0.3">
@@ -98210,7 +98213,7 @@
         <v>2</v>
       </c>
       <c r="F3999" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4000" spans="1:6" x14ac:dyDescent="0.3">
@@ -98230,7 +98233,7 @@
         <v>2</v>
       </c>
       <c r="F4000" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4001" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>